<commit_message>
updated residential unit user appliance and hot water profiles
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_UnitUserType.xlsx
+++ b/projects/test_building/input/ID_UnitUserType.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0401FF-54BB-3A4E-A67E-135C89959864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BAC119-A192-E74A-A357-C8F3A2FDF3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15480" yWindow="-18980" windowWidth="17500" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -391,10 +391,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
tables updated for new unit user type definition
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_UnitUserType.xlsx
+++ b/projects/test_building/input/ID_UnitUserType.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BAC119-A192-E74A-A357-C8F3A2FDF3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B667C056-A2A5-A144-A81F-C2C712519ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15480" yWindow="-18980" windowWidth="17500" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,36 +31,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>single fully-employed adult household</t>
-  </si>
-  <si>
-    <t>single non-working adult household</t>
-  </si>
-  <si>
-    <t>two fully-employed adults household</t>
-  </si>
-  <si>
-    <t>two non-working adults household</t>
-  </si>
-  <si>
-    <t>two fully-employed adults and two children household</t>
-  </si>
-  <si>
-    <t>two fully-employed adults and one child household</t>
-  </si>
-  <si>
-    <t>one fully-employed adult and one non-working adult household</t>
-  </si>
-  <si>
     <t>company for all tertiary sectors</t>
   </si>
   <si>
     <t>id_unit_user_type</t>
+  </si>
+  <si>
+    <t>single person household</t>
+  </si>
+  <si>
+    <t>couple without resident child</t>
+  </si>
+  <si>
+    <t>couple with resident child(ren)</t>
+  </si>
+  <si>
+    <t>single parent with resident child(ren)</t>
+  </si>
+  <si>
+    <t>other household</t>
   </si>
 </sst>
 </file>
@@ -116,8 +110,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B9" totalsRowShown="0">
-  <autoFilter ref="A1:B9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_unit_user_type"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
@@ -389,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -403,7 +397,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -414,7 +408,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -422,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -430,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -438,7 +432,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -454,23 +448,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>